<commit_message>
chnages in Index.xlsx not saved before last closure of the file. No changes recorded.
</commit_message>
<xml_diff>
--- a/Index.xlsx
+++ b/Index.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mippolimi-my.sharepoint.com/personal/claudio_paliotta_gsom_polimi_it/Documents/100_Business_Transformation_Club/Indicators/Streamlit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8CDB0455-13C8-594D-9D46-0EE46E5E5704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{8CDB0455-13C8-594D-9D46-0EE46E5E5704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5524960C-09A6-D348-B467-74D123F13BEB}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" activeTab="1" xr2:uid="{A9B17A0C-BA8E-094D-AAE9-816B331FA0BE}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" activeTab="2" xr2:uid="{A9B17A0C-BA8E-094D-AAE9-816B331FA0BE}"/>
   </bookViews>
   <sheets>
     <sheet name="GFC quarterly" sheetId="1" r:id="rId1"/>
@@ -456,7 +456,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0.##########"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -512,6 +512,14 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -604,10 +612,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -724,8 +733,10 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -22529,8 +22540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B18F88C-9067-4249-B794-3E73A8F5AD86}">
   <dimension ref="B2:AF55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P62" sqref="P62"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="N43" sqref="N43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -25866,7 +25877,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9CF6431-FCB5-7340-8FAF-457FEEB493A4}">
   <dimension ref="B2:AB42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -25918,7 +25929,7 @@
       <c r="B5" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="42" t="s">
         <v>102</v>
       </c>
       <c r="Q5" s="36"/>
@@ -28609,6 +28620,9 @@
   <mergeCells count="1">
     <mergeCell ref="Q3:V7"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C5" r:id="rId1" xr:uid="{1A440EFF-B66C-8542-922F-9B1EBBF8B164}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -35379,8 +35393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28E29F32-FCF9-EE48-9DE9-F16ACC764C53}">
   <dimension ref="A2:AD42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12:M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>